<commit_message>
Completamento Progetto con multithreading
</commit_message>
<xml_diff>
--- a/data/374500/benchmark/MongoDB.xlsx
+++ b/data/374500/benchmark/MongoDB.xlsx
@@ -451,38 +451,38 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
         <v>18</v>
       </c>
       <c r="D3" t="n">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="n">
         <v>13</v>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="D4" t="n">
         <v>24</v>
@@ -490,27 +490,27 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
         <v>25</v>
@@ -518,27 +518,27 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="n">
         <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D8" t="n">
         <v>24</v>
@@ -546,16 +546,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -563,18 +563,18 @@
         <v>7</v>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" t="n">
         <v>13</v>
@@ -583,35 +583,35 @@
         <v>18</v>
       </c>
       <c r="D11" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="n">
         <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
         <v>18</v>
       </c>
       <c r="D13" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
@@ -619,10 +619,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" t="n">
         <v>24</v>
@@ -630,13 +630,13 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="D15" t="n">
         <v>24</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" t="n">
         <v>12</v>
@@ -653,15 +653,15 @@
         <v>18</v>
       </c>
       <c r="D16" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" t="n">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C17" t="n">
         <v>18</v>
@@ -672,13 +672,13 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="n">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="D18" t="n">
         <v>24</v>
@@ -686,44 +686,44 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C19" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" t="n">
         <v>13</v>
       </c>
       <c r="C20" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C21" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D21" t="n">
-        <v>25</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22">
@@ -731,10 +731,10 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D22" t="n">
         <v>24</v>
@@ -742,7 +742,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B23" t="n">
         <v>12</v>
@@ -751,7 +751,7 @@
         <v>18</v>
       </c>
       <c r="D23" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
@@ -759,13 +759,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D24" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25">
@@ -773,10 +773,10 @@
         <v>6</v>
       </c>
       <c r="B25" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D25" t="n">
         <v>23</v>
@@ -784,13 +784,13 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B26" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C26" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D26" t="n">
         <v>24</v>
@@ -801,13 +801,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D27" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28">
@@ -815,35 +815,35 @@
         <v>7</v>
       </c>
       <c r="B28" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D28" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" t="n">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="D29" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" t="n">
         <v>19</v>
@@ -854,21 +854,21 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D31" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="n">
         <v>13</v>
@@ -877,7 +877,7 @@
         <v>20</v>
       </c>
       <c r="D32" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -923,69 +923,69 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B2" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C2" t="n">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D2" t="n">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B3" t="n">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="C3" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" t="n">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B4" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D4" t="n">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="B5" t="n">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5" t="n">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D5" t="n">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B6" t="n">
         <v>89</v>
       </c>
       <c r="C6" t="n">
-        <v>212</v>
+        <v>128</v>
       </c>
       <c r="D6" t="n">
         <v>172</v>
@@ -993,97 +993,97 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7" t="n">
-        <v>134</v>
+        <v>92</v>
       </c>
       <c r="C7" t="n">
-        <v>130</v>
+        <v>225</v>
       </c>
       <c r="D7" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" t="n">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="C8" t="n">
         <v>129</v>
       </c>
       <c r="D8" t="n">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B9" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C9" t="n">
-        <v>207</v>
+        <v>129</v>
       </c>
       <c r="D9" t="n">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B10" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C10" t="n">
-        <v>130</v>
+        <v>223</v>
       </c>
       <c r="D10" t="n">
-        <v>299</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C11" t="n">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D11" t="n">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B12" t="n">
+        <v>90</v>
+      </c>
+      <c r="C12" t="n">
         <v>131</v>
       </c>
-      <c r="C12" t="n">
-        <v>204</v>
-      </c>
       <c r="D12" t="n">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B13" t="n">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="C13" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D13" t="n">
         <v>174</v>
@@ -1091,44 +1091,44 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" t="n">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D14" t="n">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B15" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" t="n">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D15" t="n">
-        <v>289</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>43</v>
+        <v>151</v>
       </c>
       <c r="B16" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C16" t="n">
-        <v>209</v>
+        <v>134</v>
       </c>
       <c r="D16" t="n">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17">
@@ -1136,69 +1136,69 @@
         <v>45</v>
       </c>
       <c r="B17" t="n">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C17" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D17" t="n">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B18" t="n">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="C18" t="n">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D18" t="n">
-        <v>298</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B19" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C19" t="n">
-        <v>208</v>
+        <v>130</v>
       </c>
       <c r="D19" t="n">
-        <v>173</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C20" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D20" t="n">
-        <v>171</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B21" t="n">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C21" t="n">
-        <v>130</v>
+        <v>226</v>
       </c>
       <c r="D21" t="n">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22">
@@ -1206,10 +1206,10 @@
         <v>47</v>
       </c>
       <c r="B22" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C22" t="n">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D22" t="n">
         <v>172</v>
@@ -1217,27 +1217,27 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B23" t="n">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="C23" t="n">
-        <v>213</v>
+        <v>141</v>
       </c>
       <c r="D23" t="n">
-        <v>296</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B24" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C24" t="n">
-        <v>131</v>
+        <v>238</v>
       </c>
       <c r="D24" t="n">
         <v>171</v>
@@ -1245,86 +1245,86 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B25" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C25" t="n">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D25" t="n">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B26" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C26" t="n">
-        <v>210</v>
+        <v>144</v>
       </c>
       <c r="D26" t="n">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>47</v>
+        <v>147</v>
       </c>
       <c r="B27" t="n">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="C27" t="n">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D27" t="n">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B28" t="n">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="C28" t="n">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D28" t="n">
-        <v>296</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B29" t="n">
-        <v>85</v>
+        <v>189</v>
       </c>
       <c r="C29" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D29" t="n">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" t="n">
         <v>90</v>
       </c>
       <c r="C30" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D30" t="n">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31">
@@ -1332,24 +1332,24 @@
         <v>44</v>
       </c>
       <c r="B31" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C31" t="n">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D31" t="n">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B32" t="n">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C32" t="n">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="D32" t="n">
         <v>170</v>
@@ -1398,436 +1398,436 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>295</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>138</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>202</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>201</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>233</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>297</v>
       </c>
       <c r="D5" t="n">
-        <v>124</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>207</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>204</v>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>304</v>
       </c>
       <c r="D8" t="n">
-        <v>6</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>211</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>239</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>206</v>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>137</v>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>309</v>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>208</v>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>138</v>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>297</v>
       </c>
       <c r="D13" t="n">
-        <v>7</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>137</v>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D14" t="n">
-        <v>7</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>245</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="D15" t="n">
-        <v>7</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>135</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>300</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>349</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="D17" t="n">
-        <v>7</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>235</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="D18" t="n">
-        <v>7</v>
+        <v>342</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C19" t="n">
-        <v>5</v>
+        <v>301</v>
       </c>
       <c r="D19" t="n">
-        <v>7</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>212</v>
       </c>
       <c r="D20" t="n">
-        <v>7</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2</v>
+        <v>178</v>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="C21" t="n">
-        <v>5</v>
+        <v>206</v>
       </c>
       <c r="D21" t="n">
-        <v>7</v>
+        <v>353</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="B22" t="n">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>304</v>
       </c>
       <c r="D22" t="n">
-        <v>7</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>240</v>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>234</v>
       </c>
       <c r="D23" t="n">
-        <v>7</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="B24" t="n">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>214</v>
       </c>
       <c r="D24" t="n">
-        <v>7</v>
+        <v>353</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>131</v>
       </c>
       <c r="C25" t="n">
-        <v>6</v>
+        <v>336</v>
       </c>
       <c r="D25" t="n">
-        <v>8</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>237</v>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="D26" t="n">
-        <v>7</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="C27" t="n">
-        <v>6</v>
+        <v>316</v>
       </c>
       <c r="D27" t="n">
-        <v>7</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>137</v>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>334</v>
       </c>
       <c r="D28" t="n">
-        <v>7</v>
+        <v>354</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B29" t="n">
-        <v>4</v>
+        <v>135</v>
       </c>
       <c r="C29" t="n">
-        <v>5</v>
+        <v>221</v>
       </c>
       <c r="D29" t="n">
-        <v>7</v>
+        <v>356</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="B30" t="n">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="C30" t="n">
-        <v>6</v>
+        <v>328</v>
       </c>
       <c r="D30" t="n">
-        <v>7</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B31" t="n">
-        <v>4</v>
+        <v>239</v>
       </c>
       <c r="C31" t="n">
-        <v>5</v>
+        <v>216</v>
       </c>
       <c r="D31" t="n">
-        <v>7</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2</v>
+        <v>175</v>
       </c>
       <c r="B32" t="n">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="D32" t="n">
-        <v>7</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -1873,436 +1873,436 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>197</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>254</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>275</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>384</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>181</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>287</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>259</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>186</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>195</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>260</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>198</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>407</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>287</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>259</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="B8" t="n">
-        <v>127</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>199</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>385</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B9" t="n">
-        <v>180</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>200</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>255</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B10" t="n">
-        <v>189</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>283</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>257</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="B11" t="n">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>396</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="B12" t="n">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>259</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="B13" t="n">
-        <v>144</v>
+        <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>276</v>
+        <v>5</v>
       </c>
       <c r="D13" t="n">
-        <v>380</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="B14" t="n">
-        <v>179</v>
+        <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>285</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>258</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B15" t="n">
-        <v>183</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>202</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>254</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="B16" t="n">
-        <v>137</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>201</v>
+        <v>5</v>
       </c>
       <c r="D16" t="n">
-        <v>381</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="B17" t="n">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>281</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>256</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="B18" t="n">
-        <v>143</v>
+        <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>195</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>254</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B19" t="n">
-        <v>176</v>
+        <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>196</v>
+        <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>395</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>86</v>
+        <v>2</v>
       </c>
       <c r="B20" t="n">
-        <v>176</v>
+        <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>276</v>
+        <v>6</v>
       </c>
       <c r="D20" t="n">
-        <v>256</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="B21" t="n">
-        <v>181</v>
+        <v>4</v>
       </c>
       <c r="C21" t="n">
-        <v>293</v>
+        <v>6</v>
       </c>
       <c r="D21" t="n">
-        <v>384</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="B22" t="n">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D22" t="n">
-        <v>262</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="B23" t="n">
-        <v>131</v>
+        <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>198</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>259</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="B24" t="n">
-        <v>172</v>
+        <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>286</v>
+        <v>7</v>
       </c>
       <c r="D24" t="n">
-        <v>395</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="B25" t="n">
-        <v>177</v>
+        <v>4</v>
       </c>
       <c r="C25" t="n">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>258</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="B26" t="n">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>198</v>
+        <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>381</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="B27" t="n">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>282</v>
+        <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>255</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="B28" t="n">
-        <v>133</v>
+        <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>252</v>
+        <v>6</v>
       </c>
       <c r="D28" t="n">
-        <v>254</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="B29" t="n">
-        <v>172</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>203</v>
+        <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>388</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="B30" t="n">
-        <v>177</v>
+        <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>279</v>
+        <v>6</v>
       </c>
       <c r="D30" t="n">
-        <v>255</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="B31" t="n">
-        <v>179</v>
+        <v>4</v>
       </c>
       <c r="C31" t="n">
-        <v>287</v>
+        <v>6</v>
       </c>
       <c r="D31" t="n">
-        <v>373</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="B32" t="n">
-        <v>126</v>
+        <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>198</v>
+        <v>6</v>
       </c>
       <c r="D32" t="n">
-        <v>257</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifica Neo4JWriter migliorato e Neo4JBench
</commit_message>
<xml_diff>
--- a/data/374500/benchmark/MongoDB.xlsx
+++ b/data/374500/benchmark/MongoDB.xlsx
@@ -448,30 +448,30 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
         <v>5</v>
       </c>
       <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
         <v>7</v>
-      </c>
-      <c r="D2" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -479,10 +479,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -496,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -504,13 +504,13 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -524,10 +524,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -538,10 +538,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -549,27 +549,27 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -577,13 +577,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -594,7 +594,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -605,10 +605,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -616,16 +616,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -633,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
         <v>2</v>
@@ -664,7 +664,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
@@ -672,13 +672,13 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="n">
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
         <v>2</v>
@@ -686,16 +686,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -706,24 +706,24 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -731,13 +731,13 @@
         <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="n">
         <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -748,24 +748,24 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -776,10 +776,10 @@
         <v>2</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -790,38 +790,38 @@
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -832,10 +832,10 @@
         <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -846,10 +846,10 @@
         <v>2</v>
       </c>
       <c r="C30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -857,13 +857,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -874,10 +874,10 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -929,7 +929,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
@@ -940,41 +940,41 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -985,21 +985,21 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
@@ -1010,10 +1010,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
         <v>2</v>
@@ -1021,16 +1021,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1038,10 +1038,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
@@ -1055,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
         <v>2</v>
@@ -1063,13 +1063,13 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
         <v>2</v>
@@ -1077,13 +1077,13 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="n">
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>2</v>
@@ -1091,13 +1091,13 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
         <v>2</v>
@@ -1105,13 +1105,13 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="n">
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" t="n">
         <v>2</v>
@@ -1122,24 +1122,24 @@
         <v>2</v>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="n">
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
         <v>2</v>
@@ -1147,30 +1147,30 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="n">
         <v>2</v>
       </c>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1181,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D20" t="n">
         <v>2</v>
@@ -1189,13 +1189,13 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="n">
         <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
         <v>2</v>
@@ -1209,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
         <v>2</v>
@@ -1217,30 +1217,30 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="n">
         <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1248,27 +1248,27 @@
         <v>2</v>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="n">
         <v>2</v>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -1279,24 +1279,24 @@
         <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" t="n">
         <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1307,38 +1307,38 @@
         <v>2</v>
       </c>
       <c r="C29" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" t="n">
         <v>2</v>
       </c>
       <c r="C30" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D30" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="n">
         <v>2</v>
       </c>
       <c r="C31" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1346,13 +1346,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1398,142 +1398,142 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C2" t="n">
-        <v>302</v>
+        <v>117</v>
       </c>
       <c r="D2" t="n">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B3" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" t="n">
-        <v>278</v>
+        <v>102</v>
       </c>
       <c r="D3" t="n">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B4" t="n">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C4" t="n">
-        <v>294</v>
+        <v>119</v>
       </c>
       <c r="D4" t="n">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B5" t="n">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C5" t="n">
-        <v>307</v>
+        <v>132</v>
       </c>
       <c r="D5" t="n">
-        <v>180</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B6" t="n">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C6" t="n">
-        <v>318</v>
+        <v>116</v>
       </c>
       <c r="D6" t="n">
-        <v>182</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B7" t="n">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C7" t="n">
-        <v>319</v>
+        <v>117</v>
       </c>
       <c r="D7" t="n">
-        <v>163</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B8" t="n">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C8" t="n">
-        <v>270</v>
+        <v>110</v>
       </c>
       <c r="D8" t="n">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C9" t="n">
-        <v>266</v>
+        <v>113</v>
       </c>
       <c r="D9" t="n">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" t="n">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C10" t="n">
-        <v>304</v>
+        <v>111</v>
       </c>
       <c r="D10" t="n">
-        <v>182</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B11" t="n">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C11" t="n">
-        <v>275</v>
+        <v>116</v>
       </c>
       <c r="D11" t="n">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12">
@@ -1541,111 +1541,111 @@
         <v>27</v>
       </c>
       <c r="B12" t="n">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C12" t="n">
-        <v>291</v>
+        <v>112</v>
       </c>
       <c r="D12" t="n">
-        <v>153</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C13" t="n">
-        <v>319</v>
+        <v>135</v>
       </c>
       <c r="D13" t="n">
-        <v>146</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C14" t="n">
-        <v>323</v>
+        <v>116</v>
       </c>
       <c r="D14" t="n">
-        <v>172</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B15" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C15" t="n">
-        <v>266</v>
+        <v>110</v>
       </c>
       <c r="D15" t="n">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B16" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" t="n">
-        <v>300</v>
+        <v>116</v>
       </c>
       <c r="D16" t="n">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" t="n">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C17" t="n">
-        <v>346</v>
+        <v>108</v>
       </c>
       <c r="D17" t="n">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B18" t="n">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C18" t="n">
-        <v>336</v>
+        <v>108</v>
       </c>
       <c r="D18" t="n">
-        <v>184</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C19" t="n">
-        <v>342</v>
+        <v>108</v>
       </c>
       <c r="D19" t="n">
-        <v>159</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20">
@@ -1653,181 +1653,181 @@
         <v>34</v>
       </c>
       <c r="B20" t="n">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C20" t="n">
-        <v>280</v>
+        <v>112</v>
       </c>
       <c r="D20" t="n">
-        <v>164</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B21" t="n">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C21" t="n">
-        <v>305</v>
+        <v>110</v>
       </c>
       <c r="D21" t="n">
-        <v>169</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C22" t="n">
-        <v>273</v>
+        <v>111</v>
       </c>
       <c r="D22" t="n">
-        <v>184</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B23" t="n">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" t="n">
-        <v>285</v>
+        <v>121</v>
       </c>
       <c r="D23" t="n">
-        <v>199</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B24" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C24" t="n">
-        <v>259</v>
+        <v>119</v>
       </c>
       <c r="D24" t="n">
-        <v>246</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C25" t="n">
-        <v>288</v>
+        <v>102</v>
       </c>
       <c r="D25" t="n">
-        <v>250</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B26" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C26" t="n">
-        <v>284</v>
+        <v>109</v>
       </c>
       <c r="D26" t="n">
-        <v>453</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B27" t="n">
         <v>66</v>
       </c>
       <c r="C27" t="n">
-        <v>312</v>
+        <v>104</v>
       </c>
       <c r="D27" t="n">
-        <v>518</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C28" t="n">
-        <v>340</v>
+        <v>116</v>
       </c>
       <c r="D28" t="n">
-        <v>433</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B29" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C29" t="n">
-        <v>240</v>
+        <v>105</v>
       </c>
       <c r="D29" t="n">
-        <v>474</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B30" t="n">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C30" t="n">
-        <v>268</v>
+        <v>120</v>
       </c>
       <c r="D30" t="n">
-        <v>615</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B31" t="n">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C31" t="n">
-        <v>329</v>
+        <v>107</v>
       </c>
       <c r="D31" t="n">
-        <v>573</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C32" t="n">
-        <v>244</v>
+        <v>116</v>
       </c>
       <c r="D32" t="n">
-        <v>654</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1879,21 +1879,21 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -1907,10 +1907,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1921,10 +1921,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1932,10 +1932,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -1949,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -1957,16 +1957,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1977,10 +1977,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1991,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -2002,10 +2002,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -2019,7 +2019,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -2027,13 +2027,13 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -2041,13 +2041,13 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -2055,13 +2055,13 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -2069,13 +2069,13 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -2083,27 +2083,27 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -2117,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
@@ -2131,7 +2131,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
         <v>1</v>
@@ -2142,13 +2142,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -2159,10 +2159,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -2173,10 +2173,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -2187,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
@@ -2201,10 +2201,10 @@
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -2215,24 +2215,24 @@
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -2240,13 +2240,13 @@
         <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -2257,10 +2257,10 @@
         <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -2271,24 +2271,24 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="n">
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -2299,10 +2299,10 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>